<commit_message>
Refactor flashcard UI for improved layout and integrate Flowbite for enhanced styling
</commit_message>
<xml_diff>
--- a/flashcards.xlsx
+++ b/flashcards.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Studies\STADIO\FLASHCARDS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DF295D5-D72C-4124-8141-8F0693D5C381}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEA1E517-06C0-4CBD-B8E7-608D6B8FBCF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{D4189E40-F43F-474D-B5F4-BDE2A4B97CD2}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>Question</t>
   </si>
@@ -59,121 +59,61 @@
     <t>What is Computer Engineering and what are typical specializations?</t>
   </si>
   <si>
-    <t>Information Technology (IT) is the use of computers to enable humans to create, store, process and retrieve information, encompassing hardware (e.g. PCs, servers), software (e.g. applications, operating systems), networks (e.g. LANs, WANs) and services that support these functions.</t>
-  </si>
-  <si>
     <t>Explain how Information Technology (IT) enhances human productivity in everyday life.</t>
   </si>
   <si>
-    <t>IT enhances productivity by automating routine tasks (e.g. spreadsheets for budgeting); providing instant access to information (e.g. email, search engines); enabling collaboration (e.g. cloud document sharing); and supporting creativity (e.g. digital design tools).</t>
-  </si>
-  <si>
     <t>Compare and contrast Information Technology (IT) and Computer Science (CS).</t>
   </si>
   <si>
-    <t>• IT applies and manages computing technologies to solve practical problems (e.g. network configuration, system administration); • Computer Science (CS) focuses on the theoretical foundations of computation and the design of algorithms, data structures and programming languages.</t>
-  </si>
-  <si>
-    <t>Computer Science (CS) is the study of algorithms, data structures, programming languages, artificial intelligence (AI) and the theoretical foundations of hardware and software systems.</t>
-  </si>
-  <si>
-    <t>Software Engineering (SE) is the disciplined, engineering-based approach to the systematic design, development, testing and maintenance of software applications using principles such as requirements analysis, design patterns and project management.</t>
-  </si>
-  <si>
     <t>Compare Computer Science (CS) versus Software Engineering (SE).</t>
   </si>
   <si>
-    <t>• CS emphasizes theoretical aspects of computation (e.g. algorithms, computation theory); • SE emphasizes practical application of engineering principles to build, test and maintain large-scale software systems (e.g. the Software Development Life Cycle, testing, version control).</t>
-  </si>
-  <si>
     <t>Define Information System (IS) and list its main components.</t>
   </si>
   <si>
-    <t>An Information System (IS) is a collection of hardware, software, data, people and networks designed to collect, process, store and disseminate information for a specific purpose; main components are Hardware (e.g. servers, routers); Software (e.g. applications, operating systems); Data (raw facts and processed information); People (end users and IT staff); Networks (communication links).</t>
-  </si>
-  <si>
     <t>List and briefly describe three common types of Information Systems (IS).</t>
   </si>
   <si>
-    <t>• Transaction Processing System (TPS): automates routine business transactions (e.g. point-of-sale terminals); • Management Information System (MIS): generates reports and dashboards for management decision-making (e.g. monthly sales summaries); • Decision Support System (DSS): provides analytical tools and models to support complex decisions (e.g. what-if scenario simulations).</t>
-  </si>
-  <si>
-    <t>Cognitive Science is the interdisciplinary study of how the human brain perceives, learns and stores information; informed by Psychology (mental processes), Neuroscience (brain function), Linguistics (language processing), Artificial Intelligence (AI) and Philosophy (mind and knowledge).</t>
-  </si>
-  <si>
-    <t>Computer Engineering blends electrical engineering and computer science to design and implement computer hardware and low-level software; typical specializations include Embedded Systems (hardware-software integration for dedicated devices), Very Large-Scale Integration (VLSI) design (integrated circuits), and Networking (LAN/WAN and wireless communication systems).</t>
-  </si>
-  <si>
-    <t>Explain the three measures of central tendency and their appropriate use cases.</t>
-  </si>
-  <si>
-    <t>• Mean (average): sum of values divided by count; best for symmetric distributions; • Median: middle value in ordered data; robust to outliers, use for skewed distributions; • Mode: most frequent value; useful for categorical data or when distribution is multimodal.</t>
-  </si>
-  <si>
-    <t>Describe the differences between bar graphs, line graphs, and circle (pie) charts.</t>
-  </si>
-  <si>
-    <t>• Bar graphs compare quantities across categories using bars; • Line graphs connect data points to show trends over time or continuous variables; • Circle (pie) charts show proportions of a whole by dividing a circle into slices.</t>
-  </si>
-  <si>
-    <t>List and briefly describe five key milestones in the history of computing technology between 1792 and 1989.</t>
-  </si>
-  <si>
-    <t>• 1792–1871: Charles Babbage’s Difference Engine design; • 1815: Ada Lovelace publishes the first algorithm for a machine; • 1888: Herman Hollerith’s punch-card tabulator for the US census; • 1946: ENIAC (Electronic Numerical Integrator and Computer) commissioned as the first large-scale electronic digital computer; • 1989: Tim Berners-Lee develops the World Wide Web (WWW).</t>
-  </si>
-  <si>
-    <t>Define microprocessor and discuss its historical significance.</t>
-  </si>
-  <si>
-    <t>A microprocessor is an integrated circuit containing the functions of a CPU on a single chip; introduced in 1971 (Intel 4004), it enabled the miniaturization of computers into personal devices, spurred the personal-computer revolution and fostered innovation in software, gaming and networking.</t>
-  </si>
-  <si>
-    <t>Explain the role of ARPANET (Advanced Research Projects Agency Network) in the development of the Internet.</t>
-  </si>
-  <si>
-    <t>ARPANET, launched in 1969 by the US Department of Defense, was the first packet-switched network; it demonstrated reliable long-distance data routing, introduced protocols (e.g. NCP evolving into TCP/IP) and became the technical core of today’s Internet backbone.</t>
-  </si>
-  <si>
-    <t>Identify and discuss the three generations of human-computer interfaces.</t>
-  </si>
-  <si>
-    <t>• Command-Line Interfaces (CLI) (1950s–1970s): text-only, powerful but steep learning curve; • Graphical User Interfaces (GUI) (1980s): windows, icons, menus and pointers, made computing accessible; • Web and Mobile Interfaces (1990s–present): hypertext browsers, touchscreens and voice assistants, enabling ubiquitous and intuitive interaction.</t>
-  </si>
-  <si>
-    <t>Explain the difference between the Internet and the World Wide Web (WWW).</t>
-  </si>
-  <si>
-    <t>The Internet is the global network infrastructure of interconnected routers and servers using TCP/IP to transport all forms of data; the World Wide Web (WWW) is a service running over the Internet that uses HTTP/HTTPS to access hypertext documents (web pages) via browsers.</t>
-  </si>
-  <si>
-    <t>Discuss one positive and one negative social impact of computing technology since the mid-20th century.</t>
-  </si>
-  <si>
-    <t>Positive: enhanced communication—email and instant messaging enable real-time global collaboration; Negative: rise of cybercrime, including malware, identity theft and online fraud, creating new security challenges.</t>
-  </si>
-  <si>
-    <t>Describe the significance of the IBM Personal Computer (PC) introduction in 1981 on personal computing.</t>
-  </si>
-  <si>
-    <t>The IBM PC standardized open hardware architecture, leading to an explosion of “IBM-compatible” clones that drove down prices, fostered a broad software ecosystem (DOS and early Windows) and shifted computing from mainframes to desktops in homes and small businesses.</t>
-  </si>
-  <si>
-    <t>Explain how the Hollerith tabulating machine influenced modern computing systems.</t>
-  </si>
-  <si>
-    <t>Hollerith’s punch-card tabulator (1888) automated large-scale data processing for the US census, introduced data encoding and machine-readable storage, spawned the company that became IBM and established batch-processing design patterns still used in enterprise systems.</t>
-  </si>
-  <si>
-    <t>Create an ordered list of at least four landmark firsts in computing history with dates.</t>
-  </si>
-  <si>
-    <t>1. 1792: Babbage’s Difference Engine design; 2. 1815: Ada Lovelace’s algorithm publication; 3. 1946: ENIAC commissioned; 4. 1971: Intel 4004 microprocessor released; 5. 1989: Berners-Lee writes first WWW code.</t>
-  </si>
-  <si>
-    <t>Discuss how the evolution of user interfaces has enabled broader adoption of computing technologies.</t>
-  </si>
-  <si>
-    <t>Evolution from text-based CLIs to GUIs and then to web/mobile/touch/voice interfaces lowered technical skill requirements, expanded computing into education, healthcare and retail, and paved the way for mobile and Internet of Things (IoT) devices in everyday life.</t>
+    <t>Information Technology (IT) is the use of computers to make humans more productive by allowing them to create, store, process and retrieve information. It encompasses hardware, software, networks and services that enable these functions.</t>
+  </si>
+  <si>
+    <t>- It automates routine tasks such as spreadsheets for budgets - It provides instant access to information through email and search engines - It enables collaboration via cloud document sharing - It supports creativity with digital design tools</t>
+  </si>
+  <si>
+    <t>- Information Technology (IT) focuses on applying and managing computing technologies to solve practical problems such as installing networks and configuring systems - Computer Science (CS) focuses on the theory and design of algorithms, data structures and software, for example writing new programming languages and researching artificial intelligence</t>
+  </si>
+  <si>
+    <t>Computer Science (CS) is the study of algorithms, data structures, programming languages, artificial intelligence and machine learning, as well as the theoretical foundations of computing hardware and software.</t>
+  </si>
+  <si>
+    <t>Software Engineering (SE) is the disciplined, engineering-based approach to designing, developing, testing and maintaining software applications using principles of engineering, best-practice design and programming languages to build reliable, scalable software for end users.</t>
+  </si>
+  <si>
+    <t>- Computer Science (CS) emphasizes theoretical foundations such as algorithms and computation theory - Software Engineering (SE) emphasizes the practical application of engineering principles to build and maintain large software systems, including software development lifecycle, testing and project management</t>
+  </si>
+  <si>
+    <t>Information System (IS) is a collection of hardware, software, data, people and networks designed to collect, process, store and disseminate information for a specific purpose. - Hardware: PCs, servers, routers - Software: applications, operating systems - Data: raw facts and processed information - People: users and IT staff - Networks: communication links</t>
+  </si>
+  <si>
+    <t>- Transaction Processing System (TPS): automates routine business transactions such as point-of-sale - Management Information System (MIS): provides reports and dashboards for decision making such as monthly sales summaries - Decision Support System (DSS): offers analytical tools and models to support complex decisions such as what-if scenario analysis</t>
+  </si>
+  <si>
+    <t>Cognitive Science is the study of how the human brain perceives, learns and stores information. It draws on Psychology (mental processes), Neuroscience (brain function) and Linguistics (language processing).</t>
+  </si>
+  <si>
+    <t>Computer Engineering blends electrical engineering and computer science to design and implement computer hardware and low-level software. Typical specializations include embedded systems for dedicated devices, very-large-scale integration (VLSI) for designing integrated circuits and networking for designing local and wide area communication systems.</t>
+  </si>
+  <si>
+    <t>Explain the measures of central tendency and when to use each.</t>
+  </si>
+  <si>
+    <t>- Mean: sum of values divided by number of values, used for symmetric distributions - Median: middle value when data are ordered, robust against outliers, used when data are skewed - Mode: most frequent value, used for categorical data or multimodal distributions</t>
+  </si>
+  <si>
+    <t>Describe the differences between bar graphs, line graphs and pie charts.</t>
+  </si>
+  <si>
+    <t>- Bar graph: uses vertical or horizontal bars to compare quantities across categories - Line graph: connects data points to show trends over time or continuous variables - Pie chart: divides a circle into slices representing proportions of a whole, used to show percentage breakdowns of a single variable</t>
   </si>
 </sst>
 </file>
@@ -564,8 +504,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4169C2F-9B89-4909-972B-682C7C22D63F}">
   <dimension ref="A1:B39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -582,71 +522,71 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" ht="72" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="72" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
-        <v>10</v>
-      </c>
       <c r="B4" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="72" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="72" x14ac:dyDescent="0.3">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>5</v>
       </c>
@@ -654,7 +594,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>6</v>
       </c>
@@ -670,7 +610,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="72" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>24</v>
       </c>
@@ -678,85 +618,45 @@
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="A14" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A15" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A16" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A17" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A18" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" ht="72" x14ac:dyDescent="0.3">
-      <c r="A19" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A20" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A21" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A22" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A23" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>45</v>
-      </c>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" s="2"/>
+      <c r="B14" s="1"/>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" s="2"/>
+      <c r="B15" s="2"/>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" s="2"/>
+      <c r="B16" s="2"/>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" s="2"/>
+      <c r="B17" s="2"/>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" s="2"/>
+      <c r="B18" s="2"/>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" s="2"/>
+      <c r="B19" s="2"/>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" s="2"/>
+      <c r="B20" s="2"/>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" s="2"/>
+      <c r="B21" s="2"/>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22" s="2"/>
+      <c r="B22" s="2"/>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23" s="2"/>
+      <c r="B23" s="2"/>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" s="2"/>

</xml_diff>